<commit_message>
Switch to Excel View
</commit_message>
<xml_diff>
--- a/CARDS/Excel/template.xlsx
+++ b/CARDS/Excel/template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\CARDS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8BA3B2-AA8F-4B35-BD18-06EBA3FC133A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C37323B-2033-4C03-86B0-E528CC1A96E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23448" yWindow="2460" windowWidth="15504" windowHeight="16656" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
+    <workbookView xWindow="17940" yWindow="4536" windowWidth="15504" windowHeight="16656" activeTab="1" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Card" sheetId="1" r:id="rId1"/>
+    <sheet name="Website" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Task List</t>
+  </si>
+  <si>
+    <t>Have your design printed at Vista Print.</t>
+  </si>
+  <si>
+    <t>Use your new cards.</t>
+  </si>
+  <si>
+    <t>Browse our collection of card designs.</t>
+  </si>
+  <si>
+    <t>Pick out your favorite.</t>
+  </si>
   <si>
     <t>David W. Knight</t>
   </si>
   <si>
     <t>503-975-5544</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Text "Cards" to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>971-236-1579</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Get your design personalized for only $40.</t>
+  </si>
+  <si>
+    <t>Earn $20 for each of your referrals!</t>
   </si>
 </sst>
 </file>
@@ -51,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,33 +115,66 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="26"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,25 +189,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,16 +251,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1508760</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>335280</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1775460</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -187,12 +289,17 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="449580" y="830580"/>
-          <a:ext cx="1059180" cy="1059180"/>
+          <a:off x="3032760" y="1424940"/>
+          <a:ext cx="1287780" cy="1287780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+        </a:ln>
         <a:effectLst>
           <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
             <a:prstClr val="black">
@@ -524,139 +631,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E638810B-CA41-4111-9EB3-48F32535F78F}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="B1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="37.109375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+    </row>
+    <row r="5" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="10"/>
+    </row>
+    <row r="6" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+    </row>
+    <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="10"/>
+    </row>
+    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFABC4B-B73A-4823-BE7B-6D82B4B4DECE}">
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33.6" x14ac:dyDescent="0.65">
-      <c r="A1" s="4" t="s">
+    <row r="2" spans="1:3" ht="47.4" x14ac:dyDescent="0.9">
+      <c r="A2" s="1"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="5">
-        <f t="shared" ref="A4:A19" si="0">A3 * 2</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="5">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5">
-        <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5">
-        <f t="shared" si="0"/>
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5">
-        <f t="shared" si="0"/>
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5">
-        <f t="shared" si="0"/>
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5">
-        <f t="shared" si="0"/>
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A13" s="3">
-        <f t="shared" si="0"/>
-        <v>20480</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A14" s="3">
-        <f t="shared" si="0"/>
-        <v>40960</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="3">
-        <f t="shared" si="0"/>
-        <v>81920</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="3">
-        <f t="shared" si="0"/>
-        <v>163840</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A17" s="3">
-        <f t="shared" si="0"/>
-        <v>327680</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>655360</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="21" x14ac:dyDescent="0.4">
-      <c r="A19" s="3">
-        <f t="shared" si="0"/>
-        <v>1310720</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Custom folder and rebecca's card.
</commit_message>
<xml_diff>
--- a/CARDS/Excel/template.xlsx
+++ b/CARDS/Excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\CARDS\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\BlinDesigners\CARDS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9623882C-5160-44B9-AA63-3ACB00F557C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FF3C84-23A0-4C97-800A-31572B2CBD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17940" yWindow="4536" windowWidth="15504" windowHeight="16656" activeTab="1" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
+    <workbookView xWindow="12915" yWindow="3675" windowWidth="32505" windowHeight="26280" activeTab="1" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <t>I am designing creative custom calling cards.</t>
   </si>
   <si>
-    <t>Cards that are worth up to $20 each!</t>
+    <t>You get $20 for each new customer!</t>
   </si>
 </sst>
 </file>
@@ -170,7 +170,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="18"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -669,54 +668,54 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="37.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="37.109375" style="6"/>
+    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="37.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="24" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -730,29 +729,29 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="62.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" ht="47.4" x14ac:dyDescent="0.9">
+    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A2" s="1"/>
       <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -761,7 +760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="4">
         <v>2</v>
@@ -770,7 +769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -779,7 +778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -788,7 +787,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
         <v>9</v>
@@ -797,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
         <v>10</v>
@@ -806,7 +805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="D9" s="14"/>
     </row>
@@ -818,5 +817,6 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7123AE11-6237-4684-89C2-1C695D616FE8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lot's of clean up.  New featurs added to HTML template.
</commit_message>
<xml_diff>
--- a/CARDS/Excel/template.xlsx
+++ b/CARDS/Excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\BlinDesigners\CARDS\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\CARDS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FF3C84-23A0-4C97-800A-31572B2CBD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B9A6C8-F2C1-4597-ACC0-A646DFDCCA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12915" yWindow="3675" windowWidth="32505" windowHeight="26280" activeTab="1" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
+    <workbookView xWindow="19656" yWindow="1524" windowWidth="15504" windowHeight="16656" activeTab="1" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -80,13 +80,13 @@
     <t>Cards that direct people here via QR code.</t>
   </si>
   <si>
-    <t>Cards that create new customers!</t>
-  </si>
-  <si>
     <t>I am designing creative custom calling cards.</t>
   </si>
   <si>
     <t>You get $20 for each new customer!</t>
+  </si>
+  <si>
+    <t>Your cards can create new customers!</t>
   </si>
 </sst>
 </file>
@@ -251,14 +251,14 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,54 +668,54 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="37.140625" style="6"/>
+    <col min="1" max="1" width="4.44140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="37.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:3" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="24" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
     </row>
-    <row r="7" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="9"/>
     </row>
-    <row r="11" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="2:3" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="2:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -729,29 +729,29 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="62.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:4" ht="47.4" x14ac:dyDescent="0.9">
       <c r="A2" s="1"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16"/>
-    </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -760,16 +760,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -778,34 +778,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="D9" s="14"/>
     </row>

</xml_diff>

<commit_message>
Use Card #1 as banner.
</commit_message>
<xml_diff>
--- a/CARDS/Excel/template.xlsx
+++ b/CARDS/Excel/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Blindesigners\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub Repositories\BlinDesigners\CARDS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC44346-43D2-4403-8DBC-E85676C8706B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF496842-6E06-49E0-9D51-4C2EF00FB785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19656" yWindow="1536" windowWidth="15504" windowHeight="21120" activeTab="2" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
+    <workbookView xWindow="19410" yWindow="3285" windowWidth="32505" windowHeight="26280" xr2:uid="{BE9F42BC-5970-4CE2-8E20-E3337A34CC05}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>Get Yourself Some Cards!</t>
-  </si>
-  <si>
-    <t>Scan The QR Code</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>You are here because someone gave you a card.</t>
   </si>
@@ -67,19 +61,22 @@
     <t>You scanned a QR code. The System Works.</t>
   </si>
   <si>
+    <t>Your Name</t>
+  </si>
+  <si>
+    <t>Your Number</t>
+  </si>
+  <si>
+    <t>You get $25 for each new customer, starting with #3.</t>
+  </si>
+  <si>
+    <t>Every $25 that you receive can double…</t>
+  </si>
+  <si>
+    <t>Scan Me</t>
+  </si>
+  <si>
     <t>This card may be worth $25!</t>
-  </si>
-  <si>
-    <t>Your Name</t>
-  </si>
-  <si>
-    <t>Your Number</t>
-  </si>
-  <si>
-    <t>You get $25 for each new customer, starting with #3.</t>
-  </si>
-  <si>
-    <t>Every $25 that you receive can double…</t>
   </si>
 </sst>
 </file>
@@ -89,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +95,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -131,21 +121,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="9" tint="-0.249977111117893"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
@@ -158,6 +133,43 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -192,61 +204,64 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="6" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -271,15 +286,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1013460</xdr:colOff>
+      <xdr:colOff>1642110</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2903220</xdr:colOff>
+      <xdr:colOff>3531870</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>426720</xdr:rowOff>
+      <xdr:rowOff>474345</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -308,8 +323,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1318260" y="1630680"/>
-          <a:ext cx="1889760" cy="1889760"/>
+          <a:off x="1946910" y="1657350"/>
+          <a:ext cx="1889760" cy="1884045"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -333,15 +348,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>187779</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2797629</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>3483429</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -356,8 +371,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1379220" y="5258889"/>
-          <a:ext cx="1730829" cy="2048691"/>
+          <a:off x="2057400" y="4826454"/>
+          <a:ext cx="1730829" cy="4374696"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst/>
@@ -710,83 +725,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E638810B-CA41-4111-9EB3-48F32535F78F}">
   <dimension ref="B1:C20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="37.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="37.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="57.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="37.109375" style="5"/>
+    <col min="1" max="1" width="4.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="77" style="15" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="37.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="47.4" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+    <row r="1" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:3" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="2:3" s="7" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+    </row>
+    <row r="6" spans="2:3" s="7" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="2:3" s="7" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8"/>
-    </row>
-    <row r="5" spans="2:3" s="10" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="2:3" s="10" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="2:3" s="10" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9"/>
-      <c r="C7" s="11"/>
-    </row>
-    <row r="8" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:3" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="2:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="2:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:2" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
+    <row r="9" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+    </row>
+    <row r="14" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:3" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" ht="41.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:2" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" ht="41.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:2" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -801,114 +814,114 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="73.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="63" x14ac:dyDescent="1.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="63.75" x14ac:dyDescent="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
-        <v>3</v>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18">
+    <row r="10" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
         <f>B9*2</f>
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18">
+    <row r="11" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
         <f t="shared" ref="B11:B15" si="0">B10*2</f>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
+    <row r="12" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18">
+    <row r="13" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="18">
+    <row r="14" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18">
+    <row r="15" spans="1:3" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="15" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" s="9" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="7"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="21" spans="1:3" s="3" customFormat="1" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="21" spans="1:3" s="3" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
     </row>
@@ -922,32 +935,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A88A212-6528-4258-B47F-98B4D9AC5A3C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.4">
+      <c r="A1" s="6"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="63" x14ac:dyDescent="1.2">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" ht="63.75" x14ac:dyDescent="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="17" t="s">
-        <v>3</v>
+      <c r="B2" s="11" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="C3" s="7"/>
+    <row r="3" spans="1:3" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>